<commit_message>
myCV folder is added
</commit_message>
<xml_diff>
--- a/Technical requirements - Fall 2019.xlsx
+++ b/Technical requirements - Fall 2019.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\poco\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -76,39 +84,52 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -118,59 +139,56 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -360,28 +378,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.29"/>
-    <col customWidth="1" min="2" max="2" width="99.57"/>
-    <col customWidth="1" min="3" max="3" width="12.29"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="99.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +438,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>HYPERLINK("https://www.cerfi.ch/","CeRFI SA")</f>
         <v>CeRFI SA</v>
@@ -432,7 +453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>HYPERLINK("https://www.monito.com/","Monito")</f>
         <v>Monito</v>
@@ -447,7 +468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>HYPERLINK("https://www.liip.ch/fr","Liip")</f>
         <v>Liip</v>
@@ -462,7 +483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>HYPERLINK("https://www.serial.ch/en/","SERIAL SA")</f>
         <v>SERIAL SA</v>
@@ -477,7 +498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -491,7 +512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="str">
         <f>HYPERLINK("https://www.msf.org/","Médecins Sans Frontières")</f>
         <v>Médecins Sans Frontières</v>
@@ -506,7 +527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="str">
         <f>HYPERLINK("https://www.gva.ch/fr/","Aéroport Genève")</f>
         <v>Aéroport Genève</v>
@@ -521,7 +542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="str">
         <f>HYPERLINK("https://coteries.com/","Coteries")</f>
         <v>Coteries</v>
@@ -536,7 +557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="str">
         <f>HYPERLINK("https://www.mindmaze.com/","MindMaze")</f>
         <v>MindMaze</v>
@@ -551,10 +572,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>HYPERLINK("https://www.berneyassocies.com/","Berney Associés ")</f>
-        <v>Berney Associés </v>
+        <v xml:space="preserve">Berney Associés </v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
@@ -566,7 +587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>HYPERLINK("https://www.johnsoncontrols.com/","Johnson Controls")</f>
         <v>Johnson Controls</v>
@@ -582,6 +603,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>